<commit_message>
Commit anterior à aula de exercícios
</commit_message>
<xml_diff>
--- a/messy_data_alocacao.xlsx
+++ b/messy_data_alocacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romul\Desktop\Trabalho\r-intermediario-mquinho2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CFC3BA-F22F-464B-915B-41823B80E819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDD44FB-143E-4D58-8156-C3DCA858065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5011D7C5-9B20-47FD-BE66-7FA01643EEA6}"/>
   </bookViews>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309C44E6-BF56-4EE6-8D6B-578EB3707FC6}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>